<commit_message>
updated sprint burndown charts, names were mixed and added names to actual user story points burned
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/Sprint_Burndown_1.xlsx
+++ b/teamOverview/sprintBacklog/Sprint_Burndown_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/392e16b045ef5b88/Documents/ComSci/Year 3 Sem 1/cscc01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\OneDrive\Documents\ComSci\Year 3 Sem 1\cscc01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{71C63D40-2589-41B0-A409-ABD911D3BAF2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1C5F9FD8-6C0F-461E-A14C-014C4E3077AF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Provisional</t>
   </si>
@@ -33,6 +33,9 @@
     <t>Task</t>
   </si>
   <si>
+    <t>3a</t>
+  </si>
+  <si>
     <t>Wed</t>
   </si>
   <si>
@@ -87,6 +90,21 @@
     <t>Burndown Chart</t>
   </si>
   <si>
+    <t>1, 3a</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>3, 6</t>
+  </si>
+  <si>
+    <t>3, 8</t>
+  </si>
+  <si>
     <t>Philip:1</t>
   </si>
   <si>
@@ -99,6 +117,12 @@
     <t>Susan:1</t>
   </si>
   <si>
+    <t>Susan:3</t>
+  </si>
+  <si>
+    <t>Riaz:3</t>
+  </si>
+  <si>
     <t>Dann:3</t>
   </si>
   <si>
@@ -114,59 +138,59 @@
     <t>Story Points</t>
   </si>
   <si>
+    <t>David:3</t>
+  </si>
+  <si>
+    <t>David:2</t>
+  </si>
+  <si>
+    <t>Riaz:2</t>
+  </si>
+  <si>
     <t>Total:</t>
   </si>
   <si>
-    <t>5a</t>
-  </si>
-  <si>
-    <t>5b</t>
-  </si>
-  <si>
-    <t>10a</t>
-  </si>
-  <si>
-    <t>10b</t>
-  </si>
-  <si>
-    <t>10c</t>
-  </si>
-  <si>
-    <t>David:1</t>
-  </si>
-  <si>
-    <t>Susan:0</t>
-  </si>
-  <si>
-    <t>Dann:1</t>
-  </si>
-  <si>
-    <t>1, 3a</t>
-  </si>
-  <si>
-    <t>Susan:3</t>
-  </si>
-  <si>
-    <t>David:0</t>
-  </si>
-  <si>
-    <t>Riaz:0</t>
-  </si>
-  <si>
-    <t>4a</t>
-  </si>
-  <si>
-    <t>Riaz:2</t>
+    <t>Tasks</t>
   </si>
   <si>
     <t>Actual User Story Points Burned</t>
+  </si>
+  <si>
+    <t>1-Philip</t>
+  </si>
+  <si>
+    <t>2-Philip</t>
+  </si>
+  <si>
+    <t>3-Susan</t>
+  </si>
+  <si>
+    <t>3a-Susan</t>
+  </si>
+  <si>
+    <t>6-Riaz</t>
+  </si>
+  <si>
+    <t>6a-Dann</t>
+  </si>
+  <si>
+    <t>6b-Dann</t>
+  </si>
+  <si>
+    <t>8-Dann</t>
+  </si>
+  <si>
+    <t>9-David</t>
+  </si>
+  <si>
+    <t>13-Riaz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,12 +205,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF242729"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -209,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -222,9 +240,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,22 +420,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,22 +492,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -628,7 +643,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="33"/>
-          <c:min val="-5"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -697,7 +712,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.77269702911649651"/>
           <c:y val="1.9062798668318284E-3"/>
-          <c:w val="0.22424899622671926"/>
+          <c:w val="0.22730297088350337"/>
           <c:h val="0.1237632424659789"/>
         </c:manualLayout>
       </c:layout>
@@ -1339,8 +1354,8 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1665,11 +1680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC1BB781-C491-4243-859C-AAD93AE5F06E}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:S31"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1681,78 +1696,76 @@
     <col min="5" max="5" width="5.109375" style="1" customWidth="1"/>
     <col min="6" max="7" width="5.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="5.44140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.21875" style="1" customWidth="1"/>
     <col min="13" max="13" width="10.21875" style="1" customWidth="1"/>
     <col min="14" max="14" width="8.109375" style="1" customWidth="1"/>
-    <col min="15" max="18" width="8.88671875" style="1"/>
-    <col min="19" max="19" width="8.88671875" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
@@ -1761,44 +1774,34 @@
         <v>1</v>
       </c>
       <c r="D3" s="4">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
         <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>2</v>
       </c>
       <c r="G3" s="1">
         <f>SUM(B3:F3)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
       <c r="K3" s="1">
-        <v>4</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="M3" s="1">
         <v>2</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="S3" s="5"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -1807,112 +1810,118 @@
         <v>0</v>
       </c>
       <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" ref="G4:G7" si="0">SUM(B4:F4)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J4" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>30</v>
+      <c r="K4" s="1">
+        <v>2</v>
       </c>
       <c r="M4" s="1">
         <v>2</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J5" s="1">
         <v>1</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>31</v>
+      <c r="K5" s="1">
+        <v>3</v>
       </c>
       <c r="M5" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>3</v>
       </c>
       <c r="F6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J6" s="1">
-        <v>2</v>
-      </c>
-      <c r="K6" s="1">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="M6" s="1">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -1921,121 +1930,110 @@
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J7" s="1">
-        <v>2</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M7" s="1">
         <v>2</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <f>SUM(B3:B7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ref="C8:G8" si="1">SUM(C3:C7)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J8" s="1">
-        <v>2</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="K8" s="1">
+        <v>5</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="M8" s="1">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J9" s="1">
         <v>2</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>34</v>
+      <c r="K9" s="1">
+        <v>6</v>
       </c>
       <c r="M9" s="1">
-        <v>5</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K10" s="1">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="M10" s="1">
-        <v>8</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -2056,83 +2054,83 @@
         <v>5</v>
       </c>
       <c r="J11" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K11" s="1">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="L11" s="1">
+        <v>6</v>
       </c>
       <c r="M11" s="1">
         <v>8</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="Q11" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
         <f>G8</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F12" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G12" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H12" s="1">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J12" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K12" s="1">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="M12" s="1">
-        <v>3</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="J13" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K13" s="1">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="M13" s="1">
         <v>3</v>
       </c>
-      <c r="R13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -2152,110 +2150,199 @@
       <c r="H14" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="J14" s="1">
+        <v>4</v>
+      </c>
+      <c r="K14" s="1">
+        <v>13</v>
+      </c>
+      <c r="L14" s="1">
+        <v>6</v>
+      </c>
+      <c r="M14" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1">
-        <v>30</v>
+        <f>G8</f>
+        <v>31</v>
       </c>
       <c r="D15" s="1">
-        <f>C15-SUM(K20:K30)</f>
-        <v>30</v>
+        <f>C15-SUM(K20:K29)</f>
+        <v>29</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ref="E15:H15" si="2">D15-SUM(L20:L30)</f>
-        <v>24</v>
+        <f>D15-SUM(L20:L29)</f>
+        <v>22</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <f>E15-SUM(M20:M29)</f>
+        <v>19</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <f>F15-SUM(N20:N29)</f>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="2"/>
+        <f>G15-SUM(O20:O29)</f>
+        <v>-7</v>
+      </c>
+      <c r="J15" s="1">
+        <v>5</v>
+      </c>
+      <c r="K15" s="1">
+        <v>16</v>
+      </c>
+      <c r="L15" s="1">
+        <v>3</v>
+      </c>
+      <c r="M15" s="1">
+        <v>3</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="J16" s="1">
+        <v>6</v>
+      </c>
+      <c r="K16" s="1">
         <v>18</v>
+      </c>
+      <c r="L16" s="1">
+        <v>3</v>
+      </c>
+      <c r="M16" s="1">
+        <v>2</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J19" s="1" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J20" s="1">
-        <v>4</v>
-      </c>
-      <c r="O20" s="1">
-        <v>4</v>
+      <c r="J20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O21" s="1">
+        <v>44</v>
+      </c>
+      <c r="L21" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J22" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="L22" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L23" s="1">
-        <v>2</v>
+        <v>46</v>
+      </c>
+      <c r="N23" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L24" s="1">
+        <v>47</v>
+      </c>
+      <c r="M24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N26" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N27" s="1">
+        <v>8</v>
+      </c>
       <c r="Q27" s="4"/>
     </row>
-    <row r="31" spans="10:17" x14ac:dyDescent="0.3">
-      <c r="J31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K31" s="1">
-        <f>SUM(K20:O30)</f>
-        <v>12</v>
+    <row r="28" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O28" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N29" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="10:17" x14ac:dyDescent="0.3">
+      <c r="J30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="1">
+        <f>SUM(K20:O29)</f>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>